<commit_message>
Commit because Josh is curious
</commit_message>
<xml_diff>
--- a/hardware/boson/rev_a/pin_mapping.xlsx
+++ b/hardware/boson/rev_a/pin_mapping.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>Button</t>
   </si>
@@ -179,6 +179,9 @@
     <t>PB09</t>
   </si>
   <si>
+    <t>PA17</t>
+  </si>
+  <si>
     <t>PA20</t>
   </si>
   <si>
@@ -237,6 +240,9 @@
   </si>
   <si>
     <t>PA18</t>
+  </si>
+  <si>
+    <t>NRF_RESET</t>
   </si>
 </sst>
 </file>
@@ -554,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,7 +581,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -583,7 +589,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -591,7 +597,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -599,7 +605,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -607,7 +613,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -615,7 +621,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -671,7 +677,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -679,7 +685,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -687,7 +693,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -695,7 +701,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -775,7 +781,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -783,20 +789,20 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="B29" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" t="s">
         <v>55</v>
@@ -804,56 +810,64 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B33" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B34" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>34</v>
       </c>
-      <c r="B36" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <f>COUNTA(A2:A36)</f>
-        <v>35</v>
+      <c r="B37" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <f>COUNTA(A2:A37)</f>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>